<commit_message>
some progress on priors
</commit_message>
<xml_diff>
--- a/inputs/data/TRFMO_PARAMETERS.xlsx
+++ b/inputs/data/TRFMO_PARAMETERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\TunaMorphometrics\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C5758B-7935-4225-9F34-FD8648283D7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806C42AD-3149-4672-9A80-C5C966D316F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{57489DEB-2B7E-4C8C-87D4-4A3F6BB1B06C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{57489DEB-2B7E-4C8C-87D4-4A3F6BB1B06C}"/>
   </bookViews>
   <sheets>
     <sheet name="OFFICIAL" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800E8FDA-1990-4B28-82A7-123316560556}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0AC07DC-CB99-4655-B598-764EF1A3C9FD}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>